<commit_message>
Make real main in package miniProjet
</commit_message>
<xml_diff>
--- a/data/graphe1500.xlsx
+++ b/data/graphe1500.xlsx
@@ -16,10 +16,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4605,11 +4601,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2095049816"/>
-        <c:axId val="-2095046952"/>
+        <c:axId val="-2145620200"/>
+        <c:axId val="-2145617256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2095049816"/>
+        <c:axId val="-2145620200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4618,7 +4614,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095046952"/>
+        <c:crossAx val="-2145617256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4626,7 +4622,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095046952"/>
+        <c:axId val="-2145617256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4637,7 +4633,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095049816"/>
+        <c:crossAx val="-2145620200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4663,16 +4659,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5018,7 +5014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1497"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
       <selection sqref="A1:B1497"/>
     </sheetView>
   </sheetViews>
@@ -17002,7 +16998,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>